<commit_message>
chore: publish carecommunication IG 5.0.0
</commit_message>
<xml_diff>
--- a/ig/carecommunication/StructureDefinition-medcom-careCommunication-message.xlsx
+++ b/ig/carecommunication/StructureDefinition-medcom-careCommunication-message.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.3</t>
+    <t>5.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-23T11:28:08+00:00</t>
+    <t>2025-10-27T14:45:58+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -266,7 +266,14 @@
   </si>
   <si>
     <t>bdl-1:total only when a search or history {total.empty() or (type = 'searchset') or (type = 'history')}
-bdl-2:entry.search only when a search {entry.search.empty() or (type = 'searchset')}bdl-3:entry.request mandatory for batch/transaction/history, otherwise prohibited {entry.all(request.exists() = (%resource.type = 'batch' or %resource.type = 'transaction' or %resource.type = 'history'))}bdl-4:entry.response mandatory for batch-response/transaction-response/history, otherwise prohibited {entry.all(response.exists() = (%resource.type = 'batch-response' or %resource.type = 'transaction-response' or %resource.type = 'history'))}bdl-7:FullUrl must be unique in a bundle, or else entries with the same fullUrl must have different meta.versionId (except in history bundles) {(type = 'history') or entry.where(fullUrl.exists()).select(fullUrl&amp;resource.meta.versionId).isDistinct()}bdl-9:A document must have an identifier with a system and a value {type = 'document' implies (identifier.system.exists() and identifier.value.exists())}bdl-10:A document must have a date {type = 'document' implies (timestamp.hasValue())}bdl-11:A document must have a Composition as the first resource {type = 'document' implies entry.first().resource.is(Composition)}bdl-12:A message must have a MessageHeader as the first resource {type = 'message' implies entry.first().resource.is(MessageHeader)}medcom-messaging-1:The MessageHeader resource shall conform to medcom-messaging-messageHeader profile {entry[0].resource.conformsTo('http://medcomfhir.dk/ig/messaging/StructureDefinition/medcom-messaging-messageHeader')}medcom-messaging-2:There shall be at least one Provenance resource in a MedCom message {entry.resource.ofType(Provenance).exists()}medcom-careCommunication-1:The MessageHeader shall conform to medcom-careCommunication-messageHeader profile {entry[0].resource.conformsTo('http://medcomfhir.dk/ig/carecommunication/StructureDefinition/medcom-careCommunication-messageHeader')}medcom-careCommunication-2:Entry shall contain exactly one Patient resource {entry.where(resource.is(Patient)).count() = 1}medcom-careCommunication-4:There shall exist a practitioner given and family name when using a PractitionerRole. {entry.resource.ofType(Practitioner).name.exists()}medcom-careCommunication-3:All Provenance resources shall be of the type medcom-careCommunication-provenance profile {entry.resource.ofType(Provenance).where(meta.profile = 'http://medcomfhir.dk/ig/carecommunication/StructureDefinition/medcom-careCommunication-provenance').exists()}medcom-careCommunication-12:If a specific recipient exists, the organisation which the CareTeam or Practitioner is a part of shall be the same as the receiver organisation in the MessageHeader resource. {Bundle.entry.resource.ofType(Communication).recipient.reference.resolve().managingOrganization.reference = %resource.entry.resource.ofType(MessageHeader).destination.receiver.reference or Bundle.entry.resource.ofType(Communication).recipient.reference.resolve().organization.reference = %resource.entry.resource.ofType(MessageHeader).destination.receiver.reference or Bundle.entry.resource.ofType(Communication).recipient.exists().not()}medcom-careCommunication-11:If a specific sender exists, the organisation which the CareTeam or Practitioner is a part of shall be the same as the sender organisation in the MessageHeader resource. {Bundle.entry.resource.ofType(Communication).extension.value.reference.resolve().managingOrganization.reference = %resource.entry.resource.ofType(MessageHeader).sender.reference or Bundle.entry.resource.ofType(Communication).extension.value.reference.resolve().organization.reference = %resource.entry.resource.ofType(MessageHeader).sender.reference or Bundle.entry.resource.ofType(Communication).extension.exists().not()}medcom-careCommunication-13:All PractitionerRole resources shall have a reference to an instance of a Practitioner resource. {Bundle.entry.resource.ofType(PractitionerRole).practitioner.reference.exists()}</t>
+bdl-2:entry.search only when a search {entry.search.empty() or (type = 'searchset')}bdl-3:entry.request mandatory for batch/transaction/history, otherwise prohibited {entry.all(request.exists() = (%resource.type = 'batch' or %resource.type = 'transaction' or %resource.type = 'history'))}bdl-4:entry.response mandatory for batch-response/transaction-response/history, otherwise prohibited {entry.all(response.exists() = (%resource.type = 'batch-response' or %resource.type = 'transaction-response' or %resource.type = 'history'))}bdl-7:FullUrl must be unique in a bundle, or else entries with the same fullUrl must have different meta.versionId (except in history bundles) {(type = 'history') or entry.where(fullUrl.exists()).select(fullUrl&amp;resource.meta.versionId).isDistinct()}bdl-9:A document must have an identifier with a system and a value {type = 'document' implies (identifier.system.exists() and identifier.value.exists())}bdl-10:A document must have a date {type = 'document' implies (timestamp.hasValue())}bdl-11:A document must have a Composition as the first resource {type = 'document' implies entry.first().resource.is(Composition)}bdl-12:A message must have a MessageHeader as the first resource {type = 'message' implies entry.first().resource.is(MessageHeader)}medcom-messaging-1:The MessageHeader resource shall conform to medcom-messaging-messageHeader profile {entry[0].resource.conformsTo('http://medcomfhir.dk/ig/messaging/StructureDefinition/medcom-messaging-messageHeader')}medcom-messaging-2:There shall be at least one Provenance resource in a MedCom message {entry.resource.ofType(Provenance).exists()}medcom-careCommunication-1:The MessageHeader shall conform to medcom-careCommunication-messageHeader profile {entry[0].resource.conformsTo('http://medcomfhir.dk/ig/carecommunication/StructureDefinition/medcom-careCommunication-messageHeader')}medcom-careCommunication-2:Entry shall contain exactly one Patient resource {entry.where(resource.is(Patient)).count() = 1}medcom-careCommunication-4:There shall exist a practitioner given and family name when using a PractitionerRole. {entry.resource.ofType(Practitioner).name.exists()}medcom-careCommunication-3:All Provenance resources shall be of the type medcom-careCommunication-provenance profile {entry.resource.ofType(Provenance).all(conformsTo('http://medcomfhir.dk/ig/carecommunication/StructureDefinition/medcom-careCommunication-provenance'))}medcom-careCommunication-12:If a specific recipient is present, at least one of the organisations that the referenced CareTeam or Practitioner/PractitionerRole belongs to MUST equal the organisation referenced in MessageHeader.receiver.
+If no specific recipient is present, this rule is not evaluated. {Bundle.entry.resource.ofType(Communication).recipient.reference.resolve().managingOrganization.reference.resolve() = %resource.entry.resource.ofType(MessageHeader).destination.receiver.reference.resolve() or Bundle.entry.resource.ofType(Communication).recipient.reference.resolve().organization.reference.resolve() = %resource.entry.resource.ofType(MessageHeader).destination.receiver.reference.resolve() or Bundle.entry.resource.ofType(Communication).recipient.exists().not()}medcom-careCommunication-11:If a specific sender is present, at least one of the organisations that the
+ referenced CareTeam or Practitioner/PractitionerRole belongs to MUST equal the organisation referenced in MessageHeader.sender.
+If no specific sender extension is present, this rule is not evaluated. {Bundle.entry.resource.ofType(Communication).extension.value.reference.resolve().managingOrganization.reference.resolve()
+        = %resource.entry.resource.ofType(MessageHeader).sender.reference.resolve()
+    or Bundle.entry.resource.ofType(Communication).extension.value.reference.resolve().organization.reference.resolve()
+        = %resource.entry.resource.ofType(MessageHeader).sender.reference.resolve()
+    or Bundle.entry.resource.ofType(Communication).extension.exists().not()}medcom-careCommunication-13:All PractitionerRole resources shall have a reference to an instance of a Practitioner resource. {Bundle.entry.resource.ofType(PractitionerRole).practitioner.reference.exists()}</t>
   </si>
   <si>
     <t>N/A</t>
@@ -361,7 +368,7 @@
     <t>A human language.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
+    <t>http://hl7.org/fhir/ValueSet/languages|4.0.1</t>
   </si>
   <si>
     <t>Resource.language</t>
@@ -1185,17 +1192,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="39.0078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="39.0078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="21.21875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="33.44140625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.44140625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="18.19140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="17.66015625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="15.140625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1204,26 +1211,26 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="168.19140625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="49.01171875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="20.59375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.98046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="144.1953125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="42.01953125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="29.98828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="28.1484375" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="24.98046875" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="42.9765625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="24.1328125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="21.4140625" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="36.84375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="31.65234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3743,7 +3750,7 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>86</v>

</xml_diff>

<commit_message>
chore: publish carecommunication IG 5.0.0 (#43)
Co-authored-by: olw-medcom <olw-medcom@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ig/carecommunication/StructureDefinition-medcom-careCommunication-message.xlsx
+++ b/ig/carecommunication/StructureDefinition-medcom-careCommunication-message.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.3</t>
+    <t>5.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-23T11:28:08+00:00</t>
+    <t>2025-10-27T14:45:58+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -266,7 +266,14 @@
   </si>
   <si>
     <t>bdl-1:total only when a search or history {total.empty() or (type = 'searchset') or (type = 'history')}
-bdl-2:entry.search only when a search {entry.search.empty() or (type = 'searchset')}bdl-3:entry.request mandatory for batch/transaction/history, otherwise prohibited {entry.all(request.exists() = (%resource.type = 'batch' or %resource.type = 'transaction' or %resource.type = 'history'))}bdl-4:entry.response mandatory for batch-response/transaction-response/history, otherwise prohibited {entry.all(response.exists() = (%resource.type = 'batch-response' or %resource.type = 'transaction-response' or %resource.type = 'history'))}bdl-7:FullUrl must be unique in a bundle, or else entries with the same fullUrl must have different meta.versionId (except in history bundles) {(type = 'history') or entry.where(fullUrl.exists()).select(fullUrl&amp;resource.meta.versionId).isDistinct()}bdl-9:A document must have an identifier with a system and a value {type = 'document' implies (identifier.system.exists() and identifier.value.exists())}bdl-10:A document must have a date {type = 'document' implies (timestamp.hasValue())}bdl-11:A document must have a Composition as the first resource {type = 'document' implies entry.first().resource.is(Composition)}bdl-12:A message must have a MessageHeader as the first resource {type = 'message' implies entry.first().resource.is(MessageHeader)}medcom-messaging-1:The MessageHeader resource shall conform to medcom-messaging-messageHeader profile {entry[0].resource.conformsTo('http://medcomfhir.dk/ig/messaging/StructureDefinition/medcom-messaging-messageHeader')}medcom-messaging-2:There shall be at least one Provenance resource in a MedCom message {entry.resource.ofType(Provenance).exists()}medcom-careCommunication-1:The MessageHeader shall conform to medcom-careCommunication-messageHeader profile {entry[0].resource.conformsTo('http://medcomfhir.dk/ig/carecommunication/StructureDefinition/medcom-careCommunication-messageHeader')}medcom-careCommunication-2:Entry shall contain exactly one Patient resource {entry.where(resource.is(Patient)).count() = 1}medcom-careCommunication-4:There shall exist a practitioner given and family name when using a PractitionerRole. {entry.resource.ofType(Practitioner).name.exists()}medcom-careCommunication-3:All Provenance resources shall be of the type medcom-careCommunication-provenance profile {entry.resource.ofType(Provenance).where(meta.profile = 'http://medcomfhir.dk/ig/carecommunication/StructureDefinition/medcom-careCommunication-provenance').exists()}medcom-careCommunication-12:If a specific recipient exists, the organisation which the CareTeam or Practitioner is a part of shall be the same as the receiver organisation in the MessageHeader resource. {Bundle.entry.resource.ofType(Communication).recipient.reference.resolve().managingOrganization.reference = %resource.entry.resource.ofType(MessageHeader).destination.receiver.reference or Bundle.entry.resource.ofType(Communication).recipient.reference.resolve().organization.reference = %resource.entry.resource.ofType(MessageHeader).destination.receiver.reference or Bundle.entry.resource.ofType(Communication).recipient.exists().not()}medcom-careCommunication-11:If a specific sender exists, the organisation which the CareTeam or Practitioner is a part of shall be the same as the sender organisation in the MessageHeader resource. {Bundle.entry.resource.ofType(Communication).extension.value.reference.resolve().managingOrganization.reference = %resource.entry.resource.ofType(MessageHeader).sender.reference or Bundle.entry.resource.ofType(Communication).extension.value.reference.resolve().organization.reference = %resource.entry.resource.ofType(MessageHeader).sender.reference or Bundle.entry.resource.ofType(Communication).extension.exists().not()}medcom-careCommunication-13:All PractitionerRole resources shall have a reference to an instance of a Practitioner resource. {Bundle.entry.resource.ofType(PractitionerRole).practitioner.reference.exists()}</t>
+bdl-2:entry.search only when a search {entry.search.empty() or (type = 'searchset')}bdl-3:entry.request mandatory for batch/transaction/history, otherwise prohibited {entry.all(request.exists() = (%resource.type = 'batch' or %resource.type = 'transaction' or %resource.type = 'history'))}bdl-4:entry.response mandatory for batch-response/transaction-response/history, otherwise prohibited {entry.all(response.exists() = (%resource.type = 'batch-response' or %resource.type = 'transaction-response' or %resource.type = 'history'))}bdl-7:FullUrl must be unique in a bundle, or else entries with the same fullUrl must have different meta.versionId (except in history bundles) {(type = 'history') or entry.where(fullUrl.exists()).select(fullUrl&amp;resource.meta.versionId).isDistinct()}bdl-9:A document must have an identifier with a system and a value {type = 'document' implies (identifier.system.exists() and identifier.value.exists())}bdl-10:A document must have a date {type = 'document' implies (timestamp.hasValue())}bdl-11:A document must have a Composition as the first resource {type = 'document' implies entry.first().resource.is(Composition)}bdl-12:A message must have a MessageHeader as the first resource {type = 'message' implies entry.first().resource.is(MessageHeader)}medcom-messaging-1:The MessageHeader resource shall conform to medcom-messaging-messageHeader profile {entry[0].resource.conformsTo('http://medcomfhir.dk/ig/messaging/StructureDefinition/medcom-messaging-messageHeader')}medcom-messaging-2:There shall be at least one Provenance resource in a MedCom message {entry.resource.ofType(Provenance).exists()}medcom-careCommunication-1:The MessageHeader shall conform to medcom-careCommunication-messageHeader profile {entry[0].resource.conformsTo('http://medcomfhir.dk/ig/carecommunication/StructureDefinition/medcom-careCommunication-messageHeader')}medcom-careCommunication-2:Entry shall contain exactly one Patient resource {entry.where(resource.is(Patient)).count() = 1}medcom-careCommunication-4:There shall exist a practitioner given and family name when using a PractitionerRole. {entry.resource.ofType(Practitioner).name.exists()}medcom-careCommunication-3:All Provenance resources shall be of the type medcom-careCommunication-provenance profile {entry.resource.ofType(Provenance).all(conformsTo('http://medcomfhir.dk/ig/carecommunication/StructureDefinition/medcom-careCommunication-provenance'))}medcom-careCommunication-12:If a specific recipient is present, at least one of the organisations that the referenced CareTeam or Practitioner/PractitionerRole belongs to MUST equal the organisation referenced in MessageHeader.receiver.
+If no specific recipient is present, this rule is not evaluated. {Bundle.entry.resource.ofType(Communication).recipient.reference.resolve().managingOrganization.reference.resolve() = %resource.entry.resource.ofType(MessageHeader).destination.receiver.reference.resolve() or Bundle.entry.resource.ofType(Communication).recipient.reference.resolve().organization.reference.resolve() = %resource.entry.resource.ofType(MessageHeader).destination.receiver.reference.resolve() or Bundle.entry.resource.ofType(Communication).recipient.exists().not()}medcom-careCommunication-11:If a specific sender is present, at least one of the organisations that the
+ referenced CareTeam or Practitioner/PractitionerRole belongs to MUST equal the organisation referenced in MessageHeader.sender.
+If no specific sender extension is present, this rule is not evaluated. {Bundle.entry.resource.ofType(Communication).extension.value.reference.resolve().managingOrganization.reference.resolve()
+        = %resource.entry.resource.ofType(MessageHeader).sender.reference.resolve()
+    or Bundle.entry.resource.ofType(Communication).extension.value.reference.resolve().organization.reference.resolve()
+        = %resource.entry.resource.ofType(MessageHeader).sender.reference.resolve()
+    or Bundle.entry.resource.ofType(Communication).extension.exists().not()}medcom-careCommunication-13:All PractitionerRole resources shall have a reference to an instance of a Practitioner resource. {Bundle.entry.resource.ofType(PractitionerRole).practitioner.reference.exists()}</t>
   </si>
   <si>
     <t>N/A</t>
@@ -361,7 +368,7 @@
     <t>A human language.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
+    <t>http://hl7.org/fhir/ValueSet/languages|4.0.1</t>
   </si>
   <si>
     <t>Resource.language</t>
@@ -1185,17 +1192,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="39.0078125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="39.0078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="21.21875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="33.44140625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.44140625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="18.19140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="17.66015625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="15.140625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1204,26 +1211,26 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="168.19140625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="49.01171875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="20.59375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.98046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="144.1953125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="42.01953125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="29.98828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="28.1484375" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="24.98046875" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="42.9765625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="24.1328125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="21.4140625" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="36.84375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="31.65234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3743,7 +3750,7 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>86</v>

</xml_diff>